<commit_message>
Finished making first document for Rob
</commit_message>
<xml_diff>
--- a/Morph_Full.xlsx
+++ b/Morph_Full.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineeisen/github/oenothera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70044DE2-5019-3542-BCAB-F3F5EB04C972}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6F8BE0-AFEF-2E44-87C4-87AFB17BDDAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18620" yWindow="8880" windowWidth="27640" windowHeight="16940" xr2:uid="{C3FEDAB6-A21C-3F48-839D-681301E05D4E}"/>
   </bookViews>
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B265B212-EE52-5D49-A9EC-B6134FF47D69}">
   <dimension ref="A1:T171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="P117" sqref="P117"/>
+    <sheetView tabSelected="1" topLeftCell="F29" workbookViewId="0">
+      <selection activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4745,7 +4745,7 @@
         <v>29</v>
       </c>
       <c r="R55" s="9">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="S55" s="7">
         <v>2.2000000000000002</v>

</xml_diff>